<commit_message>
Version final para entregar
</commit_message>
<xml_diff>
--- a/datasets/generador r2.xlsx
+++ b/datasets/generador r2.xlsx
@@ -1,22 +1,28 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="11011"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/fs/proyectos/www/tp-ia2/datasets/"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{50D9659B-AE2C-E34E-9F2F-B5B9284F2ED3}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="110" windowWidth="19420" windowHeight="11020"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="35840" windowHeight="20860" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
     <sheet name="Hoja2" sheetId="2" r:id="rId2"/>
     <sheet name="Hoja3" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="125725"/>
+  <calcPr calcId="191029"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="5">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="14">
   <si>
     <t>x1</t>
   </si>
@@ -32,12 +38,39 @@
   <si>
     <t>clase</t>
   </si>
+  <si>
+    <t>Clase 1</t>
+  </si>
+  <si>
+    <t>Clase 0</t>
+  </si>
+  <si>
+    <t>X1</t>
+  </si>
+  <si>
+    <t>X2</t>
+  </si>
+  <si>
+    <t>Media</t>
+  </si>
+  <si>
+    <t>Desviación estandar</t>
+  </si>
+  <si>
+    <t>Cantidad instancias</t>
+  </si>
+  <si>
+    <t>Probabilidad a priori</t>
+  </si>
+  <si>
+    <t>Total</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -66,14 +99,28 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -120,7 +167,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -152,9 +199,27 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -186,6 +251,24 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -361,19 +444,17 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:K83"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:V81"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A45" workbookViewId="0">
-      <selection activeCell="A67" sqref="A67"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="23.7265625" customWidth="1"/>
+    <col min="1" max="1" width="12.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11">
+    <row r="1" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -383,17 +464,51 @@
       <c r="C1" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="2" spans="1:11">
+      <c r="D1" t="s">
+        <v>0</v>
+      </c>
+      <c r="E1" t="s">
+        <v>1</v>
+      </c>
+      <c r="F1" t="s">
+        <v>4</v>
+      </c>
+      <c r="Q1" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="R1" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="S1" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="T1" s="1"/>
+      <c r="U1" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="V1" s="1"/>
+    </row>
+    <row r="2" spans="1:22" ht="32" x14ac:dyDescent="0.2">
       <c r="A2">
         <f ca="1">NORMINV(RAND(),$J$3,$K$3)</f>
-        <v>1.5749426540879723</v>
+        <v>2.0685265628935929</v>
       </c>
       <c r="B2">
         <f ca="1">NORMINV(RAND(),$J$4,$K$4)</f>
-        <v>2.5410379515611918</v>
+        <v>2.8298561911350189</v>
       </c>
       <c r="C2">
+        <v>0</v>
+      </c>
+      <c r="D2">
+        <f ca="1">NORMINV(RAND(),$J$3,$K$3)</f>
+        <v>1.8869117933693782</v>
+      </c>
+      <c r="E2">
+        <f ca="1">NORMINV(RAND(),$J$4,$K$4)</f>
+        <v>4.8309777708871859</v>
+      </c>
+      <c r="F2">
         <v>0</v>
       </c>
       <c r="J2" t="s">
@@ -402,17 +517,42 @@
       <c r="K2" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="3" spans="1:11">
+      <c r="Q2" s="1"/>
+      <c r="R2" s="1"/>
+      <c r="S2" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="T2" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="U2" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="V2" s="2" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="3" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A3">
-        <f t="shared" ref="A3:A42" ca="1" si="0">NORMINV(RAND(),$J$3,$K$3)</f>
-        <v>1.7437060441395191</v>
+        <f t="shared" ref="A3:A41" ca="1" si="0">NORMINV(RAND(),$J$3,$K$3)</f>
+        <v>2.6809737848457482</v>
       </c>
       <c r="B3">
-        <f t="shared" ref="B3:B42" ca="1" si="1">NORMINV(RAND(),$J$4,$K$4)</f>
-        <v>3.1172360858675932</v>
+        <f t="shared" ref="B3:B41" ca="1" si="1">NORMINV(RAND(),$J$4,$K$4)</f>
+        <v>2.0937942142314694</v>
       </c>
       <c r="C3">
+        <v>0</v>
+      </c>
+      <c r="D3">
+        <f t="shared" ref="D3:D11" ca="1" si="2">NORMINV(RAND(),$J$3,$K$3)</f>
+        <v>2.1811532988170117</v>
+      </c>
+      <c r="E3">
+        <f t="shared" ref="E3:E11" ca="1" si="3">NORMINV(RAND(),$J$4,$K$4)</f>
+        <v>1.7129908275197567</v>
+      </c>
+      <c r="F3">
         <v>0</v>
       </c>
       <c r="H3">
@@ -427,17 +567,39 @@
       <c r="K3">
         <v>0.5</v>
       </c>
-    </row>
-    <row r="4" spans="1:11">
+      <c r="P3" t="s">
+        <v>6</v>
+      </c>
+      <c r="Q3">
+        <f>COUNTIF($C$2:$C$81,0)</f>
+        <v>40</v>
+      </c>
+      <c r="R3">
+        <f>Q3/$Q$5</f>
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="4" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A4">
         <f t="shared" ca="1" si="0"/>
-        <v>2.1916469247956365</v>
+        <v>1.817894566309717</v>
       </c>
       <c r="B4">
         <f t="shared" ca="1" si="1"/>
-        <v>3.9139067049840737</v>
+        <v>1.8956809764882696</v>
       </c>
       <c r="C4">
+        <v>0</v>
+      </c>
+      <c r="D4">
+        <f t="shared" ca="1" si="2"/>
+        <v>2.1257519540487655</v>
+      </c>
+      <c r="E4">
+        <f t="shared" ca="1" si="3"/>
+        <v>2.2241457670063514</v>
+      </c>
+      <c r="F4">
         <v>0</v>
       </c>
       <c r="H4">
@@ -452,19 +614,41 @@
       <c r="K4">
         <v>2</v>
       </c>
-    </row>
-    <row r="5" spans="1:11">
+      <c r="P4" t="s">
+        <v>5</v>
+      </c>
+      <c r="Q4">
+        <f>COUNTIF($C$2:$C$81,1)</f>
+        <v>40</v>
+      </c>
+      <c r="R4">
+        <f>Q4/$Q$5</f>
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="5" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A5">
         <f t="shared" ca="1" si="0"/>
-        <v>2.8596543275331623</v>
+        <v>2.9155379516258906</v>
       </c>
       <c r="B5">
         <f t="shared" ca="1" si="1"/>
-        <v>2.4747879374942929</v>
+        <v>2.4772132146922594</v>
       </c>
       <c r="C5">
         <v>0</v>
       </c>
+      <c r="D5">
+        <f t="shared" ca="1" si="2"/>
+        <v>2.1758404957554909</v>
+      </c>
+      <c r="E5">
+        <f t="shared" ca="1" si="3"/>
+        <v>2.6857981603191576</v>
+      </c>
+      <c r="F5">
+        <v>0</v>
+      </c>
       <c r="H5">
         <v>1</v>
       </c>
@@ -477,17 +661,39 @@
       <c r="K5">
         <v>1</v>
       </c>
-    </row>
-    <row r="6" spans="1:11">
+      <c r="P5" t="s">
+        <v>13</v>
+      </c>
+      <c r="Q5">
+        <f>SUM(Q3:Q4)</f>
+        <v>80</v>
+      </c>
+      <c r="R5">
+        <f>SUM(R3:R4)</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A6">
         <f t="shared" ca="1" si="0"/>
-        <v>2.6096351171593737</v>
+        <v>2.3949645689415058</v>
       </c>
       <c r="B6">
         <f t="shared" ca="1" si="1"/>
-        <v>5.487076814136274</v>
+        <v>6.7120950353120694</v>
       </c>
       <c r="C6">
+        <v>0</v>
+      </c>
+      <c r="D6">
+        <f t="shared" ca="1" si="2"/>
+        <v>2.2538338101893287</v>
+      </c>
+      <c r="E6">
+        <f t="shared" ca="1" si="3"/>
+        <v>3.0669074426371208</v>
+      </c>
+      <c r="F6">
         <v>0</v>
       </c>
       <c r="H6">
@@ -503,1031 +709,1176 @@
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="1:11">
+    <row r="7" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A7">
         <f t="shared" ca="1" si="0"/>
-        <v>1.8870903353355524</v>
+        <v>1.6947813440380251</v>
       </c>
       <c r="B7">
         <f t="shared" ca="1" si="1"/>
-        <v>1.0500322859497393</v>
+        <v>2.1029987248324189</v>
       </c>
       <c r="C7">
         <v>0</v>
       </c>
-    </row>
-    <row r="8" spans="1:11">
+      <c r="D7">
+        <f t="shared" ca="1" si="2"/>
+        <v>1.6768405896236254</v>
+      </c>
+      <c r="E7">
+        <f t="shared" ca="1" si="3"/>
+        <v>3.9490143458873499</v>
+      </c>
+      <c r="F7">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A8">
         <f t="shared" ca="1" si="0"/>
-        <v>1.8721052626070147</v>
+        <v>3.141420832407237</v>
       </c>
       <c r="B8">
         <f t="shared" ca="1" si="1"/>
-        <v>5.6317492914388056</v>
+        <v>4.2543744389075187</v>
       </c>
       <c r="C8">
         <v>0</v>
       </c>
-    </row>
-    <row r="9" spans="1:11">
+      <c r="D8">
+        <f t="shared" ca="1" si="2"/>
+        <v>1.6331370733505959</v>
+      </c>
+      <c r="E8">
+        <f t="shared" ca="1" si="3"/>
+        <v>4.3686585700568052</v>
+      </c>
+      <c r="F8">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A9">
         <f t="shared" ca="1" si="0"/>
-        <v>2.4050219875102514</v>
+        <v>1.2877884719481592</v>
       </c>
       <c r="B9">
         <f t="shared" ca="1" si="1"/>
-        <v>9.8481712339718364E-2</v>
+        <v>3.6029008864338863</v>
       </c>
       <c r="C9">
         <v>0</v>
       </c>
-    </row>
-    <row r="10" spans="1:11">
+      <c r="D9">
+        <f t="shared" ca="1" si="2"/>
+        <v>1.3179050785107425</v>
+      </c>
+      <c r="E9">
+        <f t="shared" ca="1" si="3"/>
+        <v>5.4850012094485283</v>
+      </c>
+      <c r="F9">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A10">
         <f t="shared" ca="1" si="0"/>
-        <v>1.9277012623652576</v>
+        <v>1.977598511009605</v>
       </c>
       <c r="B10">
         <f t="shared" ca="1" si="1"/>
-        <v>2.6270385124594684</v>
+        <v>2.9247508903807202</v>
       </c>
       <c r="C10">
         <v>0</v>
       </c>
-    </row>
-    <row r="11" spans="1:11">
+      <c r="D10">
+        <f t="shared" ca="1" si="2"/>
+        <v>1.8055940537037822</v>
+      </c>
+      <c r="E10">
+        <f t="shared" ca="1" si="3"/>
+        <v>3.2119823724910868</v>
+      </c>
+      <c r="F10">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A11">
         <f t="shared" ca="1" si="0"/>
-        <v>1.8000718409891909</v>
+        <v>1.7703499560499099</v>
       </c>
       <c r="B11">
         <f t="shared" ca="1" si="1"/>
-        <v>2.8785447148664769</v>
+        <v>2.5955087833447013</v>
       </c>
       <c r="C11">
         <v>0</v>
       </c>
-    </row>
-    <row r="12" spans="1:11">
+      <c r="D11">
+        <f t="shared" ca="1" si="2"/>
+        <v>1.2539725617989108</v>
+      </c>
+      <c r="E11">
+        <f t="shared" ca="1" si="3"/>
+        <v>3.6168018409881251</v>
+      </c>
+      <c r="F11">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A12">
         <f t="shared" ca="1" si="0"/>
-        <v>1.9871501097890523</v>
+        <v>1.9570115976510201</v>
       </c>
       <c r="B12">
         <f t="shared" ca="1" si="1"/>
-        <v>2.8355699806154577</v>
+        <v>2.2755862402887423</v>
       </c>
       <c r="C12">
         <v>0</v>
       </c>
-    </row>
-    <row r="13" spans="1:11">
+      <c r="D12">
+        <f ca="1">NORMINV(RAND(),$J$5,$K$5)</f>
+        <v>-0.31491438314948933</v>
+      </c>
+      <c r="E12">
+        <f ca="1">NORMINV(RAND(),$J$6,$K$6)</f>
+        <v>4.2295038431902912</v>
+      </c>
+      <c r="F12">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="13" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A13">
         <f t="shared" ca="1" si="0"/>
-        <v>2.4327061320439709</v>
+        <v>1.3706939964117799</v>
       </c>
       <c r="B13">
         <f t="shared" ca="1" si="1"/>
-        <v>0.86355790591702064</v>
+        <v>5.0037485279840066</v>
       </c>
       <c r="C13">
         <v>0</v>
       </c>
-    </row>
-    <row r="14" spans="1:11">
+      <c r="D13">
+        <f t="shared" ref="D13:D21" ca="1" si="4">NORMINV(RAND(),$J$5,$K$5)</f>
+        <v>-1.7981237611134606</v>
+      </c>
+      <c r="E13">
+        <f t="shared" ref="E13:E21" ca="1" si="5">NORMINV(RAND(),$J$6,$K$6)</f>
+        <v>1.1751222279748585</v>
+      </c>
+      <c r="F13">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="14" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A14">
         <f t="shared" ca="1" si="0"/>
-        <v>3.045660228501637</v>
+        <v>1.2230848128006606</v>
       </c>
       <c r="B14">
         <f t="shared" ca="1" si="1"/>
-        <v>4.0096940804304015</v>
+        <v>1.5853003182146013</v>
       </c>
       <c r="C14">
         <v>0</v>
       </c>
-    </row>
-    <row r="15" spans="1:11">
+      <c r="D14">
+        <f t="shared" ca="1" si="4"/>
+        <v>1.1181596710331805</v>
+      </c>
+      <c r="E14">
+        <f t="shared" ca="1" si="5"/>
+        <v>0.9092324487988146</v>
+      </c>
+      <c r="F14">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="15" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A15">
         <f t="shared" ca="1" si="0"/>
-        <v>2.8607165704513475</v>
+        <v>2.4554434896168584</v>
       </c>
       <c r="B15">
         <f t="shared" ca="1" si="1"/>
-        <v>3.6433792584437632</v>
+        <v>5.9153991309987379</v>
       </c>
       <c r="C15">
         <v>0</v>
       </c>
-    </row>
-    <row r="16" spans="1:11">
+      <c r="D15">
+        <f t="shared" ca="1" si="4"/>
+        <v>-1.572773193940876</v>
+      </c>
+      <c r="E15">
+        <f t="shared" ca="1" si="5"/>
+        <v>2.0672846649640571</v>
+      </c>
+      <c r="F15">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="16" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A16">
         <f t="shared" ca="1" si="0"/>
-        <v>2.1422759443535302</v>
+        <v>2.6082419342801999</v>
       </c>
       <c r="B16">
         <f t="shared" ca="1" si="1"/>
-        <v>0.880613214229931</v>
+        <v>2.1555969637536281</v>
       </c>
       <c r="C16">
         <v>0</v>
       </c>
-    </row>
-    <row r="17" spans="1:3">
+      <c r="D16">
+        <f t="shared" ca="1" si="4"/>
+        <v>-0.83010057542814719</v>
+      </c>
+      <c r="E16">
+        <f t="shared" ca="1" si="5"/>
+        <v>1.2736229859271724</v>
+      </c>
+      <c r="F16">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A17">
         <f t="shared" ca="1" si="0"/>
-        <v>1.8589466443656528</v>
+        <v>2.3194832519096407</v>
       </c>
       <c r="B17">
         <f t="shared" ca="1" si="1"/>
-        <v>5.3754727844767167</v>
+        <v>2.416001860172547</v>
       </c>
       <c r="C17">
         <v>0</v>
       </c>
-    </row>
-    <row r="18" spans="1:3">
+      <c r="D17">
+        <f t="shared" ca="1" si="4"/>
+        <v>-1.4832594772269629</v>
+      </c>
+      <c r="E17">
+        <f t="shared" ca="1" si="5"/>
+        <v>2.3286506977745143</v>
+      </c>
+      <c r="F17">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A18">
         <f t="shared" ca="1" si="0"/>
-        <v>1.7725513948701299</v>
+        <v>2.324545694638215</v>
       </c>
       <c r="B18">
         <f t="shared" ca="1" si="1"/>
-        <v>6.4779046547390013</v>
+        <v>1.8373513234447738</v>
       </c>
       <c r="C18">
         <v>0</v>
       </c>
-    </row>
-    <row r="19" spans="1:3">
+      <c r="D18">
+        <f t="shared" ca="1" si="4"/>
+        <v>0.38701991006701786</v>
+      </c>
+      <c r="E18">
+        <f t="shared" ca="1" si="5"/>
+        <v>1.3075647650339013</v>
+      </c>
+      <c r="F18">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A19">
         <f t="shared" ca="1" si="0"/>
-        <v>1.0390463209327381</v>
+        <v>2.2748587506221067</v>
       </c>
       <c r="B19">
         <f t="shared" ca="1" si="1"/>
-        <v>3.1936213481642439</v>
+        <v>6.9771584122475954</v>
       </c>
       <c r="C19">
         <v>0</v>
       </c>
-    </row>
-    <row r="20" spans="1:3">
+      <c r="D19">
+        <f t="shared" ca="1" si="4"/>
+        <v>-0.40836638031098249</v>
+      </c>
+      <c r="E19">
+        <f t="shared" ca="1" si="5"/>
+        <v>1.9648246854969187</v>
+      </c>
+      <c r="F19">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A20">
         <f t="shared" ca="1" si="0"/>
-        <v>2.8981088155913062</v>
+        <v>1.7427383047313443</v>
       </c>
       <c r="B20">
         <f t="shared" ca="1" si="1"/>
-        <v>2.0204067360853406</v>
+        <v>-1.8454174407044199</v>
       </c>
       <c r="C20">
         <v>0</v>
       </c>
-    </row>
-    <row r="21" spans="1:3">
+      <c r="D20">
+        <f t="shared" ca="1" si="4"/>
+        <v>0.28661943174221749</v>
+      </c>
+      <c r="E20">
+        <f t="shared" ca="1" si="5"/>
+        <v>1.0309295505456773</v>
+      </c>
+      <c r="F20">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A21">
         <f t="shared" ca="1" si="0"/>
-        <v>2.1188451286204892</v>
+        <v>1.68658427599426</v>
       </c>
       <c r="B21">
         <f t="shared" ca="1" si="1"/>
-        <v>2.8376079613500735</v>
+        <v>5.6092392799884205</v>
       </c>
       <c r="C21">
         <v>0</v>
       </c>
-    </row>
-    <row r="22" spans="1:3">
+      <c r="D21">
+        <f t="shared" ca="1" si="4"/>
+        <v>-1.4488520644937528</v>
+      </c>
+      <c r="E21">
+        <f t="shared" ca="1" si="5"/>
+        <v>1.7825815095891455</v>
+      </c>
+      <c r="F21">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A22">
         <f t="shared" ca="1" si="0"/>
-        <v>2.597467044905156</v>
+        <v>2.2533787506661311</v>
       </c>
       <c r="B22">
         <f t="shared" ca="1" si="1"/>
-        <v>3.1496385198230747</v>
+        <v>4.4408026773665341</v>
       </c>
       <c r="C22">
         <v>0</v>
       </c>
     </row>
-    <row r="23" spans="1:3">
+    <row r="23" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A23">
         <f t="shared" ca="1" si="0"/>
-        <v>2.5040687181339667</v>
+        <v>1.8178485358454162</v>
       </c>
       <c r="B23">
         <f t="shared" ca="1" si="1"/>
-        <v>2.4468240424570245</v>
+        <v>4.1419374117866621</v>
       </c>
       <c r="C23">
         <v>0</v>
       </c>
     </row>
-    <row r="24" spans="1:3">
+    <row r="24" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A24">
         <f t="shared" ca="1" si="0"/>
-        <v>2.0049543543149961</v>
+        <v>2.8467232750691687</v>
       </c>
       <c r="B24">
         <f t="shared" ca="1" si="1"/>
-        <v>3.7515698212458295</v>
+        <v>3.9714530706609561</v>
       </c>
       <c r="C24">
         <v>0</v>
       </c>
     </row>
-    <row r="25" spans="1:3">
+    <row r="25" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A25">
         <f t="shared" ca="1" si="0"/>
-        <v>2.4744659282074934</v>
+        <v>1.8943511044970127</v>
       </c>
       <c r="B25">
         <f t="shared" ca="1" si="1"/>
-        <v>4.7905124423885628</v>
+        <v>1.9939575944967431</v>
       </c>
       <c r="C25">
         <v>0</v>
       </c>
     </row>
-    <row r="26" spans="1:3">
+    <row r="26" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A26">
         <f t="shared" ca="1" si="0"/>
-        <v>2.0325299287397329</v>
+        <v>2.454364832454913</v>
       </c>
       <c r="B26">
         <f t="shared" ca="1" si="1"/>
-        <v>4.5061593431256695</v>
+        <v>0.79451214268081216</v>
       </c>
       <c r="C26">
         <v>0</v>
       </c>
     </row>
-    <row r="27" spans="1:3">
+    <row r="27" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A27">
         <f t="shared" ca="1" si="0"/>
-        <v>2.2242278654395129</v>
+        <v>1.7350232957092513</v>
       </c>
       <c r="B27">
         <f t="shared" ca="1" si="1"/>
-        <v>3.9869016205118273</v>
+        <v>3.9162126461458104</v>
       </c>
       <c r="C27">
         <v>0</v>
       </c>
     </row>
-    <row r="28" spans="1:3">
+    <row r="28" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A28">
         <f t="shared" ca="1" si="0"/>
-        <v>1.7397178875645785</v>
+        <v>2.9540518752145539</v>
       </c>
       <c r="B28">
         <f t="shared" ca="1" si="1"/>
-        <v>-8.0113460669052117E-2</v>
+        <v>2.5926759061479911</v>
       </c>
       <c r="C28">
         <v>0</v>
       </c>
     </row>
-    <row r="29" spans="1:3">
+    <row r="29" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A29">
         <f t="shared" ca="1" si="0"/>
-        <v>1.5947504575413112</v>
+        <v>2.6433113883451975</v>
       </c>
       <c r="B29">
         <f t="shared" ca="1" si="1"/>
-        <v>6.4589438718582413</v>
+        <v>1.5751158359262911</v>
       </c>
       <c r="C29">
         <v>0</v>
       </c>
     </row>
-    <row r="30" spans="1:3">
+    <row r="30" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A30">
         <f t="shared" ca="1" si="0"/>
-        <v>2.4962859018727395</v>
+        <v>2.1718419996324592</v>
       </c>
       <c r="B30">
         <f t="shared" ca="1" si="1"/>
-        <v>1.1532647677494583</v>
+        <v>5.2625311540825574</v>
       </c>
       <c r="C30">
         <v>0</v>
       </c>
     </row>
-    <row r="31" spans="1:3">
+    <row r="31" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A31">
         <f t="shared" ca="1" si="0"/>
-        <v>1.5755270555165224</v>
+        <v>1.8948358950976467</v>
       </c>
       <c r="B31">
         <f t="shared" ca="1" si="1"/>
-        <v>1.7608648709450816</v>
+        <v>2.8872673257650558</v>
       </c>
       <c r="C31">
         <v>0</v>
       </c>
     </row>
-    <row r="32" spans="1:3">
+    <row r="32" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A32">
         <f t="shared" ca="1" si="0"/>
-        <v>1.847388310084261</v>
+        <v>1.8082679349276529</v>
       </c>
       <c r="B32">
         <f t="shared" ca="1" si="1"/>
-        <v>4.1954535124249563</v>
+        <v>3.8771058908291938</v>
       </c>
       <c r="C32">
         <v>0</v>
       </c>
     </row>
-    <row r="33" spans="1:3">
+    <row r="33" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A33">
         <f t="shared" ca="1" si="0"/>
-        <v>1.0779612517838066</v>
+        <v>1.5672648162521499</v>
       </c>
       <c r="B33">
         <f t="shared" ca="1" si="1"/>
-        <v>1.9459111846647041</v>
+        <v>4.853559653189353</v>
       </c>
       <c r="C33">
         <v>0</v>
       </c>
     </row>
-    <row r="34" spans="1:3">
+    <row r="34" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A34">
         <f t="shared" ca="1" si="0"/>
-        <v>1.9855516572405651</v>
+        <v>2.0197462887310733</v>
       </c>
       <c r="B34">
         <f t="shared" ca="1" si="1"/>
-        <v>0.8314087993460717</v>
+        <v>5.4908828230863787</v>
       </c>
       <c r="C34">
         <v>0</v>
       </c>
     </row>
-    <row r="35" spans="1:3">
+    <row r="35" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A35">
         <f t="shared" ca="1" si="0"/>
-        <v>1.7297046401233076</v>
+        <v>2.7940233387432283</v>
       </c>
       <c r="B35">
         <f t="shared" ca="1" si="1"/>
-        <v>5.1518648651357921</v>
+        <v>5.6661096789147116</v>
       </c>
       <c r="C35">
         <v>0</v>
       </c>
     </row>
-    <row r="36" spans="1:3">
+    <row r="36" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A36">
         <f t="shared" ca="1" si="0"/>
-        <v>2.8819648013267027</v>
+        <v>2.1543258102777734</v>
       </c>
       <c r="B36">
         <f t="shared" ca="1" si="1"/>
-        <v>3.8981514948931322</v>
+        <v>0.30970154862132304</v>
       </c>
       <c r="C36">
         <v>0</v>
       </c>
     </row>
-    <row r="37" spans="1:3">
+    <row r="37" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A37">
         <f t="shared" ca="1" si="0"/>
-        <v>1.2609541001817419</v>
+        <v>1.970323883267761</v>
       </c>
       <c r="B37">
         <f t="shared" ca="1" si="1"/>
-        <v>2.4115635944604499</v>
+        <v>0.96083250003279419</v>
       </c>
       <c r="C37">
         <v>0</v>
       </c>
     </row>
-    <row r="38" spans="1:3">
+    <row r="38" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A38">
         <f t="shared" ca="1" si="0"/>
-        <v>2.4298619943451643</v>
+        <v>0.8989650760542196</v>
       </c>
       <c r="B38">
         <f t="shared" ca="1" si="1"/>
-        <v>5.0089916667780541</v>
+        <v>5.03118735144864</v>
       </c>
       <c r="C38">
         <v>0</v>
       </c>
     </row>
-    <row r="39" spans="1:3">
+    <row r="39" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A39">
         <f t="shared" ca="1" si="0"/>
-        <v>2.7706510490401377</v>
+        <v>2.4573496228527096</v>
       </c>
       <c r="B39">
         <f t="shared" ca="1" si="1"/>
-        <v>1.7508573016928595</v>
+        <v>4.6490964409607844</v>
       </c>
       <c r="C39">
         <v>0</v>
       </c>
     </row>
-    <row r="40" spans="1:3">
+    <row r="40" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A40">
         <f t="shared" ca="1" si="0"/>
-        <v>2.4643881053757934</v>
+        <v>2.1220126461844777</v>
       </c>
       <c r="B40">
         <f t="shared" ca="1" si="1"/>
-        <v>0.76303125465886978</v>
+        <v>3.6152250771634424</v>
       </c>
       <c r="C40">
         <v>0</v>
       </c>
     </row>
-    <row r="41" spans="1:3">
+    <row r="41" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A41">
         <f t="shared" ca="1" si="0"/>
-        <v>1.6048266697121121</v>
+        <v>1.7721222802565002</v>
       </c>
       <c r="B41">
         <f t="shared" ca="1" si="1"/>
-        <v>4.1828990789972735</v>
+        <v>4.744492843274684</v>
       </c>
       <c r="C41">
         <v>0</v>
       </c>
     </row>
-    <row r="42" spans="1:3">
+    <row r="42" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A42">
-        <f t="shared" ca="1" si="0"/>
-        <v>2.4402073551046959</v>
+        <f ca="1">NORMINV(RAND(),$J$5,$K$5)</f>
+        <v>0.17993363239212862</v>
       </c>
       <c r="B42">
-        <f t="shared" ca="1" si="1"/>
-        <v>3.6672615174714789</v>
+        <f ca="1">NORMINV(RAND(),$J$6,$K$6)</f>
+        <v>0.91575974780041691</v>
       </c>
       <c r="C42">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="43" spans="1:3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="43" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A43">
-        <f ca="1">NORMINV(RAND(),$J$5,$K$5)</f>
-        <v>1.078748799128022</v>
+        <f t="shared" ref="A43:A81" ca="1" si="6">NORMINV(RAND(),$J$5,$K$5)</f>
+        <v>-0.21518908498033654</v>
       </c>
       <c r="B43">
-        <f ca="1">NORMINV(RAND(),$J$6,$K$6)</f>
-        <v>3.5370473611923434</v>
+        <f t="shared" ref="B43:B81" ca="1" si="7">NORMINV(RAND(),$J$6,$K$6)</f>
+        <v>2.7209587264119426</v>
       </c>
       <c r="C43">
         <v>1</v>
       </c>
     </row>
-    <row r="44" spans="1:3">
+    <row r="44" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A44">
-        <f t="shared" ref="A44:A83" ca="1" si="2">NORMINV(RAND(),$J$5,$K$5)</f>
-        <v>1.906600534829114</v>
+        <f t="shared" ca="1" si="6"/>
+        <v>-1.4325265728754866</v>
       </c>
       <c r="B44">
-        <f t="shared" ref="B44:B83" ca="1" si="3">NORMINV(RAND(),$J$6,$K$6)</f>
-        <v>2.3430179027751228</v>
+        <f t="shared" ca="1" si="7"/>
+        <v>1.0104546168703901</v>
       </c>
       <c r="C44">
         <v>1</v>
       </c>
     </row>
-    <row r="45" spans="1:3">
+    <row r="45" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A45">
-        <f t="shared" ca="1" si="2"/>
-        <v>0.41349687832114546</v>
+        <f t="shared" ca="1" si="6"/>
+        <v>-1.823257560143771</v>
       </c>
       <c r="B45">
-        <f t="shared" ca="1" si="3"/>
-        <v>0.53786480967650308</v>
+        <f t="shared" ca="1" si="7"/>
+        <v>3.2355057638525939</v>
       </c>
       <c r="C45">
         <v>1</v>
       </c>
     </row>
-    <row r="46" spans="1:3">
+    <row r="46" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A46">
-        <f t="shared" ca="1" si="2"/>
-        <v>-0.70138182987973008</v>
+        <f t="shared" ca="1" si="6"/>
+        <v>4.9135348867510503E-2</v>
       </c>
       <c r="B46">
-        <f t="shared" ca="1" si="3"/>
-        <v>2.1263243102244833</v>
+        <f t="shared" ca="1" si="7"/>
+        <v>-0.34360031014156611</v>
       </c>
       <c r="C46">
         <v>1</v>
       </c>
     </row>
-    <row r="47" spans="1:3">
+    <row r="47" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A47">
-        <f t="shared" ca="1" si="2"/>
-        <v>1.6868765848352472</v>
+        <f t="shared" ca="1" si="6"/>
+        <v>1.1802913268730768</v>
       </c>
       <c r="B47">
-        <f t="shared" ca="1" si="3"/>
-        <v>3.0008624127881238</v>
+        <f t="shared" ca="1" si="7"/>
+        <v>3.4750268736722005</v>
       </c>
       <c r="C47">
         <v>1</v>
       </c>
     </row>
-    <row r="48" spans="1:3">
+    <row r="48" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A48">
-        <f t="shared" ca="1" si="2"/>
-        <v>-4.484862941891879E-2</v>
+        <f t="shared" ca="1" si="6"/>
+        <v>-1.0266730347549866</v>
       </c>
       <c r="B48">
-        <f t="shared" ca="1" si="3"/>
-        <v>0.92199293244310399</v>
+        <f t="shared" ca="1" si="7"/>
+        <v>3.481471616233879</v>
       </c>
       <c r="C48">
         <v>1</v>
       </c>
     </row>
-    <row r="49" spans="1:3">
+    <row r="49" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A49">
-        <f t="shared" ca="1" si="2"/>
-        <v>-0.33895152286267749</v>
+        <f t="shared" ca="1" si="6"/>
+        <v>-1.8721233919638218</v>
       </c>
       <c r="B49">
-        <f t="shared" ca="1" si="3"/>
-        <v>3.320181304147332</v>
+        <f t="shared" ca="1" si="7"/>
+        <v>0.47477273687266752</v>
       </c>
       <c r="C49">
         <v>1</v>
       </c>
     </row>
-    <row r="50" spans="1:3">
+    <row r="50" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A50">
-        <f t="shared" ca="1" si="2"/>
-        <v>-0.33955445153551567</v>
+        <f t="shared" ca="1" si="6"/>
+        <v>1.025915825506488</v>
       </c>
       <c r="B50">
-        <f t="shared" ca="1" si="3"/>
-        <v>2.3262986714493343</v>
+        <f t="shared" ca="1" si="7"/>
+        <v>0.36336427526748549</v>
       </c>
       <c r="C50">
         <v>1</v>
       </c>
     </row>
-    <row r="51" spans="1:3">
+    <row r="51" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A51">
-        <f t="shared" ca="1" si="2"/>
-        <v>-0.21999941520483679</v>
+        <f t="shared" ca="1" si="6"/>
+        <v>0.98195943619070625</v>
       </c>
       <c r="B51">
-        <f t="shared" ca="1" si="3"/>
-        <v>1.1309717062447817</v>
+        <f t="shared" ca="1" si="7"/>
+        <v>1.3164338915695679</v>
       </c>
       <c r="C51">
         <v>1</v>
       </c>
     </row>
-    <row r="52" spans="1:3">
+    <row r="52" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A52">
-        <f t="shared" ca="1" si="2"/>
-        <v>-0.174880856116503</v>
+        <f t="shared" ca="1" si="6"/>
+        <v>-4.447651294254807E-2</v>
       </c>
       <c r="B52">
-        <f t="shared" ca="1" si="3"/>
-        <v>1.6324870935283007</v>
+        <f t="shared" ca="1" si="7"/>
+        <v>3.10914540407278</v>
       </c>
       <c r="C52">
         <v>1</v>
       </c>
     </row>
-    <row r="53" spans="1:3">
+    <row r="53" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A53">
-        <f t="shared" ca="1" si="2"/>
-        <v>1.1013713546617181</v>
+        <f t="shared" ca="1" si="6"/>
+        <v>0.18415703402769515</v>
       </c>
       <c r="B53">
-        <f t="shared" ca="1" si="3"/>
-        <v>3.088615853322648</v>
+        <f t="shared" ca="1" si="7"/>
+        <v>1.8329511793283328</v>
       </c>
       <c r="C53">
         <v>1</v>
       </c>
     </row>
-    <row r="54" spans="1:3">
+    <row r="54" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A54">
-        <f t="shared" ca="1" si="2"/>
-        <v>-0.78851141321735119</v>
+        <f t="shared" ca="1" si="6"/>
+        <v>-3.325312014866777</v>
       </c>
       <c r="B54">
-        <f t="shared" ca="1" si="3"/>
-        <v>0.17873172672888726</v>
+        <f t="shared" ca="1" si="7"/>
+        <v>2.0954022028579486</v>
       </c>
       <c r="C54">
         <v>1</v>
       </c>
     </row>
-    <row r="55" spans="1:3">
+    <row r="55" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A55">
-        <f t="shared" ca="1" si="2"/>
-        <v>0.39106356011599996</v>
+        <f t="shared" ca="1" si="6"/>
+        <v>-1.3282664233346329</v>
       </c>
       <c r="B55">
-        <f t="shared" ca="1" si="3"/>
-        <v>2.6215399851517498</v>
+        <f t="shared" ca="1" si="7"/>
+        <v>2.1781010417584721</v>
       </c>
       <c r="C55">
         <v>1</v>
       </c>
     </row>
-    <row r="56" spans="1:3">
+    <row r="56" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A56">
-        <f t="shared" ca="1" si="2"/>
-        <v>7.3799325612616901E-2</v>
+        <f t="shared" ca="1" si="6"/>
+        <v>0.50963205095982467</v>
       </c>
       <c r="B56">
-        <f t="shared" ca="1" si="3"/>
-        <v>0.93647952118704936</v>
+        <f t="shared" ca="1" si="7"/>
+        <v>0.25170718758652577</v>
       </c>
       <c r="C56">
         <v>1</v>
       </c>
     </row>
-    <row r="57" spans="1:3">
+    <row r="57" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A57">
-        <f t="shared" ca="1" si="2"/>
-        <v>-1.1820996714348073</v>
+        <f t="shared" ca="1" si="6"/>
+        <v>0.40747989798538009</v>
       </c>
       <c r="B57">
-        <f t="shared" ca="1" si="3"/>
-        <v>2.7308858948266637</v>
+        <f t="shared" ca="1" si="7"/>
+        <v>1.7108270968658379</v>
       </c>
       <c r="C57">
         <v>1</v>
       </c>
     </row>
-    <row r="58" spans="1:3">
+    <row r="58" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A58">
-        <f t="shared" ca="1" si="2"/>
-        <v>0.55800694351076241</v>
+        <f t="shared" ca="1" si="6"/>
+        <v>-1.2816050347717927</v>
       </c>
       <c r="B58">
-        <f t="shared" ca="1" si="3"/>
-        <v>0.46718875110624891</v>
+        <f t="shared" ca="1" si="7"/>
+        <v>1.7924057411390362</v>
       </c>
       <c r="C58">
         <v>1</v>
       </c>
     </row>
-    <row r="59" spans="1:3">
+    <row r="59" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A59">
-        <f t="shared" ca="1" si="2"/>
-        <v>-0.51261580473821522</v>
+        <f t="shared" ca="1" si="6"/>
+        <v>0.81590745789849084</v>
       </c>
       <c r="B59">
-        <f t="shared" ca="1" si="3"/>
-        <v>3.220753725255483</v>
+        <f t="shared" ca="1" si="7"/>
+        <v>0.76375061005297851</v>
       </c>
       <c r="C59">
         <v>1</v>
       </c>
     </row>
-    <row r="60" spans="1:3">
+    <row r="60" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A60">
-        <f t="shared" ca="1" si="2"/>
-        <v>-0.22729906311049936</v>
+        <f t="shared" ca="1" si="6"/>
+        <v>0.79377239056215609</v>
       </c>
       <c r="B60">
-        <f t="shared" ca="1" si="3"/>
-        <v>1.8312286288947224</v>
+        <f t="shared" ca="1" si="7"/>
+        <v>1.8719162156269553</v>
       </c>
       <c r="C60">
         <v>1</v>
       </c>
     </row>
-    <row r="61" spans="1:3">
+    <row r="61" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A61">
-        <f t="shared" ca="1" si="2"/>
-        <v>0.56245826304639124</v>
+        <f t="shared" ca="1" si="6"/>
+        <v>0.46594372806660178</v>
       </c>
       <c r="B61">
-        <f t="shared" ca="1" si="3"/>
-        <v>0.4228486339960944</v>
+        <f t="shared" ca="1" si="7"/>
+        <v>1.4431412824740129</v>
       </c>
       <c r="C61">
         <v>1</v>
       </c>
     </row>
-    <row r="62" spans="1:3">
+    <row r="62" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A62">
-        <f t="shared" ca="1" si="2"/>
-        <v>-0.78263813488648859</v>
+        <f t="shared" ca="1" si="6"/>
+        <v>-0.1481337162824598</v>
       </c>
       <c r="B62">
-        <f t="shared" ca="1" si="3"/>
-        <v>1.7275052985330466</v>
+        <f t="shared" ca="1" si="7"/>
+        <v>3.1381339398503489</v>
       </c>
       <c r="C62">
         <v>1</v>
       </c>
     </row>
-    <row r="63" spans="1:3">
+    <row r="63" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A63">
-        <f t="shared" ca="1" si="2"/>
-        <v>-0.37223461249308076</v>
+        <f t="shared" ca="1" si="6"/>
+        <v>-1.9768080597891573E-2</v>
       </c>
       <c r="B63">
-        <f t="shared" ca="1" si="3"/>
-        <v>2.5719767121927344</v>
+        <f t="shared" ca="1" si="7"/>
+        <v>1.8842007148008124</v>
       </c>
       <c r="C63">
         <v>1</v>
       </c>
     </row>
-    <row r="64" spans="1:3">
+    <row r="64" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A64">
-        <f t="shared" ca="1" si="2"/>
-        <v>-0.11559179513175583</v>
+        <f t="shared" ca="1" si="6"/>
+        <v>-0.65822295331709613</v>
       </c>
       <c r="B64">
-        <f t="shared" ca="1" si="3"/>
-        <v>2.5930511553702682</v>
+        <f t="shared" ca="1" si="7"/>
+        <v>0.60339806374679195</v>
       </c>
       <c r="C64">
         <v>1</v>
       </c>
     </row>
-    <row r="65" spans="1:3">
+    <row r="65" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A65">
-        <f t="shared" ca="1" si="2"/>
-        <v>-0.3524960631708588</v>
+        <f t="shared" ca="1" si="6"/>
+        <v>-1.2823668792336911</v>
       </c>
       <c r="B65">
-        <f t="shared" ca="1" si="3"/>
-        <v>1.1282813059951509</v>
+        <f t="shared" ca="1" si="7"/>
+        <v>2.318454528895507</v>
       </c>
       <c r="C65">
         <v>1</v>
       </c>
     </row>
-    <row r="66" spans="1:3">
+    <row r="66" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A66">
-        <f t="shared" ca="1" si="2"/>
-        <v>-1.656367165610698</v>
+        <f t="shared" ca="1" si="6"/>
+        <v>-2.1875206043792588</v>
       </c>
       <c r="B66">
-        <f t="shared" ca="1" si="3"/>
-        <v>2.0812514905628565</v>
+        <f t="shared" ca="1" si="7"/>
+        <v>2.9038988599699262</v>
       </c>
       <c r="C66">
         <v>1</v>
       </c>
     </row>
-    <row r="67" spans="1:3">
+    <row r="67" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A67">
-        <f t="shared" ca="1" si="2"/>
-        <v>0.27491761435497486</v>
+        <f t="shared" ca="1" si="6"/>
+        <v>0.15812912367371623</v>
       </c>
       <c r="B67">
-        <f t="shared" ca="1" si="3"/>
-        <v>2.6909976610377049</v>
+        <f t="shared" ca="1" si="7"/>
+        <v>3.4698045088733775</v>
       </c>
       <c r="C67">
         <v>1</v>
       </c>
     </row>
-    <row r="68" spans="1:3">
+    <row r="68" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A68">
-        <f t="shared" ca="1" si="2"/>
-        <v>0.47559959546136277</v>
+        <f t="shared" ca="1" si="6"/>
+        <v>-0.3151037448055557</v>
       </c>
       <c r="B68">
-        <f t="shared" ca="1" si="3"/>
-        <v>0.86716900439951683</v>
+        <f t="shared" ca="1" si="7"/>
+        <v>2.5929414035246414</v>
       </c>
       <c r="C68">
         <v>1</v>
       </c>
     </row>
-    <row r="69" spans="1:3">
+    <row r="69" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A69">
-        <f t="shared" ca="1" si="2"/>
-        <v>0.9033572079674328</v>
+        <f t="shared" ca="1" si="6"/>
+        <v>-2.0205729341265828</v>
       </c>
       <c r="B69">
-        <f t="shared" ca="1" si="3"/>
-        <v>1.806598969968221</v>
+        <f t="shared" ca="1" si="7"/>
+        <v>3.4076134378554164</v>
       </c>
       <c r="C69">
         <v>1</v>
       </c>
     </row>
-    <row r="70" spans="1:3">
+    <row r="70" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A70">
-        <f t="shared" ca="1" si="2"/>
-        <v>0.2580857505506603</v>
+        <f t="shared" ca="1" si="6"/>
+        <v>0.15714339599949298</v>
       </c>
       <c r="B70">
-        <f t="shared" ca="1" si="3"/>
-        <v>2.1703672520613448E-2</v>
+        <f t="shared" ca="1" si="7"/>
+        <v>3.1589646513069729</v>
       </c>
       <c r="C70">
         <v>1</v>
       </c>
     </row>
-    <row r="71" spans="1:3">
+    <row r="71" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A71">
-        <f t="shared" ca="1" si="2"/>
-        <v>-0.13351539514763244</v>
+        <f t="shared" ca="1" si="6"/>
+        <v>-1.636845579911042</v>
       </c>
       <c r="B71">
-        <f t="shared" ca="1" si="3"/>
-        <v>1.2228814276637581</v>
+        <f t="shared" ca="1" si="7"/>
+        <v>3.3405818841604153</v>
       </c>
       <c r="C71">
         <v>1</v>
       </c>
     </row>
-    <row r="72" spans="1:3">
+    <row r="72" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A72">
-        <f t="shared" ca="1" si="2"/>
-        <v>-0.2034949203331215</v>
+        <f t="shared" ca="1" si="6"/>
+        <v>0.85213946550099506</v>
       </c>
       <c r="B72">
-        <f t="shared" ca="1" si="3"/>
-        <v>0.17159438329801846</v>
+        <f t="shared" ca="1" si="7"/>
+        <v>1.6160478952897579</v>
       </c>
       <c r="C72">
         <v>1</v>
       </c>
     </row>
-    <row r="73" spans="1:3">
+    <row r="73" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A73">
-        <f t="shared" ca="1" si="2"/>
-        <v>1.4928854217993974</v>
+        <f t="shared" ca="1" si="6"/>
+        <v>-0.47373368208427458</v>
       </c>
       <c r="B73">
-        <f t="shared" ca="1" si="3"/>
-        <v>2.5411994917550924</v>
+        <f t="shared" ca="1" si="7"/>
+        <v>1.1605854449706141</v>
       </c>
       <c r="C73">
         <v>1</v>
       </c>
     </row>
-    <row r="74" spans="1:3">
+    <row r="74" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A74">
-        <f t="shared" ca="1" si="2"/>
-        <v>-0.56784142683094951</v>
+        <f t="shared" ca="1" si="6"/>
+        <v>0.7177882556365548</v>
       </c>
       <c r="B74">
-        <f t="shared" ca="1" si="3"/>
-        <v>1.9816292701864262</v>
+        <f t="shared" ca="1" si="7"/>
+        <v>1.463671381834585</v>
       </c>
       <c r="C74">
         <v>1</v>
       </c>
     </row>
-    <row r="75" spans="1:3">
+    <row r="75" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A75">
-        <f t="shared" ca="1" si="2"/>
-        <v>0.71987173467173227</v>
+        <f t="shared" ca="1" si="6"/>
+        <v>-1.4037085945172474</v>
       </c>
       <c r="B75">
-        <f t="shared" ca="1" si="3"/>
-        <v>2.4791032954082697</v>
+        <f t="shared" ca="1" si="7"/>
+        <v>2.5201951593759304</v>
       </c>
       <c r="C75">
         <v>1</v>
       </c>
     </row>
-    <row r="76" spans="1:3">
+    <row r="76" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A76">
-        <f t="shared" ca="1" si="2"/>
-        <v>-0.18085647652471804</v>
+        <f t="shared" ca="1" si="6"/>
+        <v>1.4847401384989387</v>
       </c>
       <c r="B76">
-        <f t="shared" ca="1" si="3"/>
-        <v>2.0732636114429726</v>
+        <f t="shared" ca="1" si="7"/>
+        <v>1.4402719845363969</v>
       </c>
       <c r="C76">
         <v>1</v>
       </c>
     </row>
-    <row r="77" spans="1:3">
+    <row r="77" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A77">
-        <f t="shared" ca="1" si="2"/>
-        <v>0.77730401950612849</v>
+        <f t="shared" ca="1" si="6"/>
+        <v>-0.17393584108320048</v>
       </c>
       <c r="B77">
-        <f t="shared" ca="1" si="3"/>
-        <v>3.6570599989851043</v>
+        <f t="shared" ca="1" si="7"/>
+        <v>0.69565955428188819</v>
       </c>
       <c r="C77">
         <v>1</v>
       </c>
     </row>
-    <row r="78" spans="1:3">
+    <row r="78" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A78">
-        <f t="shared" ca="1" si="2"/>
-        <v>-0.38421315335234563</v>
+        <f t="shared" ca="1" si="6"/>
+        <v>0.38967307294563058</v>
       </c>
       <c r="B78">
-        <f t="shared" ca="1" si="3"/>
-        <v>2.7531418975796984</v>
+        <f t="shared" ca="1" si="7"/>
+        <v>2.8001898936852023</v>
       </c>
       <c r="C78">
         <v>1</v>
       </c>
     </row>
-    <row r="79" spans="1:3">
+    <row r="79" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A79">
-        <f t="shared" ca="1" si="2"/>
-        <v>1.3714248780701568</v>
+        <f t="shared" ca="1" si="6"/>
+        <v>0.26672004211259082</v>
       </c>
       <c r="B79">
-        <f t="shared" ca="1" si="3"/>
-        <v>0.23448389447971163</v>
+        <f t="shared" ca="1" si="7"/>
+        <v>2.4663201053239532</v>
       </c>
       <c r="C79">
         <v>1</v>
       </c>
     </row>
-    <row r="80" spans="1:3">
+    <row r="80" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A80">
-        <f t="shared" ca="1" si="2"/>
-        <v>6.4385636634332111E-2</v>
+        <f t="shared" ca="1" si="6"/>
+        <v>-0.481889570765417</v>
       </c>
       <c r="B80">
-        <f t="shared" ca="1" si="3"/>
-        <v>2.6283877332352463</v>
+        <f t="shared" ca="1" si="7"/>
+        <v>1.037169144963634</v>
       </c>
       <c r="C80">
         <v>1</v>
       </c>
     </row>
-    <row r="81" spans="1:3">
+    <row r="81" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A81">
-        <f t="shared" ca="1" si="2"/>
-        <v>0.47325830185271589</v>
+        <f t="shared" ca="1" si="6"/>
+        <v>0.26318698255820983</v>
       </c>
       <c r="B81">
-        <f t="shared" ca="1" si="3"/>
-        <v>2.9078786995974624</v>
+        <f t="shared" ca="1" si="7"/>
+        <v>2.3519208044659283</v>
       </c>
       <c r="C81">
         <v>1</v>
       </c>
     </row>
-    <row r="82" spans="1:3">
-      <c r="A82">
-        <f t="shared" ca="1" si="2"/>
-        <v>-0.31961477003474659</v>
-      </c>
-      <c r="B82">
-        <f t="shared" ca="1" si="3"/>
-        <v>3.5697571263487813</v>
-      </c>
-      <c r="C82">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="83" spans="1:3">
-      <c r="A83">
-        <f t="shared" ca="1" si="2"/>
-        <v>1.4719245014746387</v>
-      </c>
-      <c r="B83">
-        <f t="shared" ca="1" si="3"/>
-        <v>1.3220435673851243</v>
-      </c>
-      <c r="C83">
-        <v>1</v>
-      </c>
-    </row>
   </sheetData>
+  <mergeCells count="4">
+    <mergeCell ref="S1:T1"/>
+    <mergeCell ref="U1:V1"/>
+    <mergeCell ref="Q1:Q2"/>
+    <mergeCell ref="R1:R2"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>